<commit_message>
inicio de csv y manajger
</commit_message>
<xml_diff>
--- a/Traduccion/Traduccion.xlsx
+++ b/Traduccion/Traduccion.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TEMP\My project\Assets\Pr-ctica-CDI\Traduccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TEMP\My project (1)\Assets\Pr-ctica-CDI\Traduccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Traduccion" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>pajaros Furiosos</t>
   </si>
@@ -60,14 +60,37 @@
   </si>
   <si>
     <t>Level 3</t>
+  </si>
+  <si>
+    <t>angro</t>
+  </si>
+  <si>
+    <t>furiosao</t>
+  </si>
+  <si>
+    <t>Levelao 1</t>
+  </si>
+  <si>
+    <t>Levelao 2</t>
+  </si>
+  <si>
+    <t>Levelao 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -95,8 +118,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,18 +404,26 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
+      <selection activeCell="C4" sqref="C4:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -400,6 +432,9 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -419,6 +454,9 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -427,6 +465,9 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -435,8 +476,12 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>